<commit_message>
Bericht und Scrum Update
Bericht erstellen, Scrum Excel Sheet einige Priorisierung verändern.
</commit_message>
<xml_diff>
--- a/doc/task-04/Scrum/scrum_group_white_2019.xlsx
+++ b/doc/task-04/Scrum/scrum_group_white_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janahansellathurai/Documents/GitHub/ch.bfh.btx8081.w2019.white/doc/task-04/Notizen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sugeelan\Documents\GitHub\ch.bfh.btx8081.w2019.white\doc\task-04\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD09AE62-6700-294F-85EF-684406810EA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5359F0-CE91-4B3C-A83A-ED25E2D3EE64}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -380,6 +380,9 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -405,7 +408,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -431,12 +437,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -512,13 +512,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3ED146B-4112-104B-B86C-671C49528323}" name="Tabelle1" displayName="Tabelle1" ref="A1:L11" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3ED146B-4112-104B-B86C-671C49528323}" name="Tabelle1" displayName="Tabelle1" ref="A1:L11" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:L11" xr:uid="{CD61C43E-D25A-5443-81A6-B90EBB9FCC84}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{68FC7359-A3EC-0A46-81A4-AF65DCEF8136}" name="ID"/>
     <tableColumn id="2" xr3:uid="{AFD358FE-B293-1B45-8566-B789BDCDA3C1}" name="Sprint"/>
-    <tableColumn id="3" xr3:uid="{EAD33B73-90D5-CD44-AC46-0DB4B4C461AC}" name="Name" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D7091834-736D-324A-8E05-E56CF91E4DB0}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EAD33B73-90D5-CD44-AC46-0DB4B4C461AC}" name="Name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D7091834-736D-324A-8E05-E56CF91E4DB0}" name="Description" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{FABE7295-8545-8A4F-864A-AE341C471F2B}" name="Components"/>
     <tableColumn id="6" xr3:uid="{E935D23C-981E-9646-8C64-6FF75273C0D8}" name="Owner"/>
     <tableColumn id="7" xr3:uid="{5BB55267-665B-5845-A754-3FAD7D8494D2}" name="Reviewer"/>
@@ -533,11 +533,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3EBABFB-B420-144F-8682-E8F5915F60C1}" name="Tabelle2" displayName="Tabelle2" ref="A1:D3" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D3" xr:uid="{789FD85D-7B9A-9D44-B030-1998E82683A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A3EBABFB-B420-144F-8682-E8F5915F60C1}" name="Tabelle2" displayName="Tabelle2" ref="A1:D57" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:D57" xr:uid="{789FD85D-7B9A-9D44-B030-1998E82683A4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{84ED6281-1169-1F43-96C2-B0CBDF80F883}" name="Sprint "/>
-    <tableColumn id="2" xr3:uid="{2C9B2C63-1CB5-2741-869E-6391B76F0E04}" name="Time of Record" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2C9B2C63-1CB5-2741-869E-6391B76F0E04}" name="Time of Record" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{DF9241F2-EED2-A644-82AD-1C2CA52106BE}" name="Remaining Effort"/>
     <tableColumn id="4" xr3:uid="{7D7B4E84-DE3A-4E44-858C-3553450F3C40}" name="Remaining Ressources"/>
   </tableColumns>
@@ -869,18 +869,18 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -891,7 +891,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -902,7 +902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -913,7 +913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -924,7 +924,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -935,7 +935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -946,7 +946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -957,7 +957,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -969,7 +969,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -981,7 +981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="6:6" ht="25" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="F18" s="4"/>
     </row>
   </sheetData>
@@ -993,24 +993,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="137" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="96" zoomScaleNormal="137" workbookViewId="0">
+      <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="5">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>8</v>
@@ -1058,7 +1058,7 @@
       <c r="J2" s="9"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1093,10 +1093,10 @@
         <v>53</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
@@ -1106,7 +1106,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="103" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1128,7 +1128,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1139,16 +1139,16 @@
         <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
         <v>5</v>
-      </c>
-      <c r="E6" s="5">
-        <v>10</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>32</v>
       </c>
@@ -1207,26 +1207,26 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1.2</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1.3</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>1.4</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1.5</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1.6</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1.7</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1.8</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2.1</v>
       </c>
@@ -1566,20 +1566,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1593,32 +1593,470 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>42262</v>
+        <v>43791</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>54</v>
       </c>
       <c r="D2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>42263</v>
-      </c>
-      <c r="C3">
-        <v>190</v>
-      </c>
-      <c r="D3">
-        <v>180</v>
+        <v>43792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43799</v>
+      </c>
+      <c r="C10">
+        <v>84</v>
+      </c>
+      <c r="D10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>43803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3">
+        <v>43805</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <v>43806</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3">
+        <v>43807</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43808</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3">
+        <v>43810</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="3">
+        <v>43813</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3">
+        <v>43814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3">
+        <v>43815</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3">
+        <v>43816</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3">
+        <v>43817</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3">
+        <v>43818</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3">
+        <v>43819</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3">
+        <v>43820</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43821</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3">
+        <v>43822</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="3">
+        <v>43823</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" s="3">
+        <v>43824</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" s="3">
+        <v>43825</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3">
+        <v>43826</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3">
+        <v>43827</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3">
+        <v>43828</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3">
+        <v>43829</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" s="3">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3">
+        <v>43832</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43833</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" s="3">
+        <v>43834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" s="3">
+        <v>43835</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" s="3">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" s="3">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" s="3">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" s="3">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" s="3">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" s="3">
+        <v>43841</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" s="3">
+        <v>43842</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" s="3">
+        <v>43843</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" s="3">
+        <v>43844</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" s="3">
+        <v>43845</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" s="3">
+        <v>43846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Scrum: wird noch weiter bearbeitet
</commit_message>
<xml_diff>
--- a/doc/task-04/Scrum/scrum_group_white_2019.xlsx
+++ b/doc/task-04/Scrum/scrum_group_white_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sugeelan\Documents\GitHub\ch.bfh.btx8081.w2019.white\doc\task-04\Scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janahansellathurai/Documents/GitHub/ch.bfh.btx8081.w2019.white/doc/task-04/Scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EC820F-AB72-4B36-A10B-37497A8254D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAD4F4C-B24D-914E-9A32-3EE916B7BA91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -319,6 +321,33 @@
 Miletic - 1.1: und 1.2 Main View, Grudngerüst - 3 Std
 Alain - 1.1: MainLayout Design und bearbeitung der Funktionen - 4 Std
 Alain - 1.8 :AppointmentView erstellt - 4 Std</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung von der Medikation</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung von den Patienten</t>
+  </si>
+  <si>
+    <t>Patientendaten genierieren</t>
+  </si>
+  <si>
+    <t>View Anpassen nach Wunsch des Product Owner</t>
+  </si>
+  <si>
+    <t>JPA-Anbindung</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Alle Klassen nach MVP implementieren</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung von Reporten</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung von Description</t>
   </si>
 </sst>
 </file>
@@ -388,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -441,13 +470,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <font>
@@ -579,8 +611,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3ED146B-4112-104B-B86C-671C49528323}" name="Tabelle1" displayName="Tabelle1" ref="A1:L11" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:L11" xr:uid="{CD61C43E-D25A-5443-81A6-B90EBB9FCC84}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3ED146B-4112-104B-B86C-671C49528323}" name="Tabelle1" displayName="Tabelle1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:L18" xr:uid="{CD61C43E-D25A-5443-81A6-B90EBB9FCC84}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{68FC7359-A3EC-0A46-81A4-AF65DCEF8136}" name="ID"/>
     <tableColumn id="2" xr3:uid="{AFD358FE-B293-1B45-8566-B789BDCDA3C1}" name="Sprint"/>
@@ -939,17 +971,17 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="16"/>
     <col min="6" max="6" width="49" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="16"/>
+    <col min="7" max="16384" width="8.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="15" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="15" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -960,7 +992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
@@ -971,7 +1003,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
@@ -982,7 +1014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>35</v>
       </c>
@@ -993,7 +1025,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>23</v>
       </c>
@@ -1004,7 +1036,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
@@ -1015,7 +1047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -1026,12 +1058,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -1043,7 +1075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
@@ -1055,7 +1087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="6:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" ht="25" x14ac:dyDescent="0.2">
       <c r="F18" s="17"/>
     </row>
   </sheetData>
@@ -1071,20 +1103,20 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1132,7 +1164,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1156,7 +1188,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1180,7 +1212,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1202,7 +1234,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1222,7 +1254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1242,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1262,7 +1294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K14" t="s">
         <v>31</v>
       </c>
@@ -1278,29 +1310,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="142" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="138" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -1377,7 +1409,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1.2</v>
       </c>
@@ -1416,7 +1448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1.3</v>
       </c>
@@ -1454,7 +1486,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1.4</v>
       </c>
@@ -1492,7 +1524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1.5</v>
       </c>
@@ -1527,7 +1559,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1.6</v>
       </c>
@@ -1565,7 +1597,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1.7</v>
       </c>
@@ -1603,7 +1635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>1.8</v>
       </c>
@@ -1641,7 +1673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2.1</v>
       </c>
@@ -1671,6 +1703,103 @@
         <v>12</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="L12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="L13" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="L14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="L15" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="L16" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="L17" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1687,19 +1816,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="138" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="52.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -1716,7 +1845,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1734,7 +1863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1752,7 +1881,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1770,7 +1899,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1788,7 +1917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1806,7 +1935,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1824,7 +1953,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1842,7 +1971,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1860,7 +1989,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1874,7 +2003,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1882,7 +2011,7 @@
         <v>43800</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1890,7 +2019,7 @@
         <v>43801</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1898,7 +2027,7 @@
         <v>43802</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1906,7 +2035,7 @@
         <v>43803</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1914,7 +2043,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1922,7 +2051,7 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1930,7 +2059,7 @@
         <v>43806</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1938,7 +2067,7 @@
         <v>43807</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1946,7 +2075,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1954,7 +2083,7 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1962,7 +2091,7 @@
         <v>43810</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1970,7 +2099,7 @@
         <v>43811</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1978,7 +2107,7 @@
         <v>43812</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1986,7 +2115,7 @@
         <v>43813</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1994,7 +2123,7 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2002,7 +2131,7 @@
         <v>43815</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2010,7 +2139,7 @@
         <v>43816</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2018,7 +2147,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2026,7 +2155,7 @@
         <v>43818</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2034,7 +2163,7 @@
         <v>43819</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2048,7 +2177,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2056,7 +2185,7 @@
         <v>43821</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2064,7 +2193,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2072,7 +2201,7 @@
         <v>43823</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2080,7 +2209,7 @@
         <v>43824</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2088,7 +2217,7 @@
         <v>43825</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2096,7 +2225,7 @@
         <v>43826</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2104,7 +2233,7 @@
         <v>43827</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2112,7 +2241,7 @@
         <v>43828</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2120,7 +2249,7 @@
         <v>43829</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2128,7 +2257,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2136,7 +2265,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2144,7 +2273,7 @@
         <v>43832</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2152,7 +2281,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2160,7 +2289,7 @@
         <v>43834</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2168,7 +2297,7 @@
         <v>43835</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2176,7 +2305,7 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2184,7 +2313,7 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2192,7 +2321,7 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2200,7 +2329,7 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2208,7 +2337,7 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2216,7 +2345,7 @@
         <v>43841</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2224,7 +2353,7 @@
         <v>43842</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2232,7 +2361,7 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2240,7 +2369,7 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2248,7 +2377,7 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
update scrum update folien
</commit_message>
<xml_diff>
--- a/doc/task-04/Scrum/scrum_group_white_2019.xlsx
+++ b/doc/task-04/Scrum/scrum_group_white_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janahansellathurai/Documents/GitHub/ch.bfh.btx8081.w2019.white/doc/task-04/Scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A9CE6D-C02F-794D-A494-3776CFCCD408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D057D-2C01-5847-B7BE-4EEC76C58512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="19660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     <t>Um unsere Applikation verwenden zu können, muss sich der Facharzt  auf der Login-View authenfizieren. Damit stellen wir sicher, dass die Patientendaten von aussen nicht für Drittpersonen sichtbar sind.</t>
   </si>
   <si>
-    <t>Der Facharzt kann seine Patiententermine auf dem Termin-View strukturiert sehen. Eintragen von zukünftigen Terminen und verwalten von eingetragenen Termine ist möglich. Die Termine werden den Patienten zugeordnet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Der Facharzt kann die Patientenstammdaten und die Patientenberichte  auf dem Patienten-View strukturiert sehen. </t>
   </si>
   <si>
@@ -539,6 +536,9 @@
 nippa1 - Koordination programierung MVP &amp; Änderung Datenbank - 8 Std 
 gaupa1 - Offene Pendenzen bei div. Klassen im Team bearbeiten - 6 Std 
 velkv1 - Offene Pendenzen bei div. Klassen im Team bearbeiten - 6 Std </t>
+  </si>
+  <si>
+    <t>Der Facharzt kann seine Patiententermine auf dem Termin-View strukturiert sehen. Die Termine werden den Patienten zugeordnet.</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3ED146B-4112-104B-B86C-671C49528323}" name="Tabelle1" displayName="Tabelle1" ref="A1:L27" totalsRowCount="1" headerRowDxfId="26">
-  <autoFilter ref="A1:L26" xr:uid="{CD61C43E-D25A-5443-81A6-B90EBB9FCC84}"/>
+  <autoFilter ref="A1:L26" xr:uid="{CD61C43E-D25A-5443-81A6-B90EBB9FCC84}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{68FC7359-A3EC-0A46-81A4-AF65DCEF8136}" name="ID" dataDxfId="25" totalsRowDxfId="24"/>
     <tableColumn id="2" xr3:uid="{AFD358FE-B293-1B45-8566-B789BDCDA3C1}" name="Sprint" dataDxfId="23" totalsRowDxfId="22"/>
@@ -1434,7 +1440,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="131" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1499,7 +1505,7 @@
         <v>59</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
@@ -1512,7 +1518,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -1530,7 +1536,7 @@
         <v>167</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="8"/>
@@ -1543,7 +1549,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>5</v>
@@ -1558,7 +1564,7 @@
         <v>25</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
@@ -1571,7 +1577,7 @@
         <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>6</v>
@@ -1586,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
@@ -1614,7 +1620,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -1625,7 +1631,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>5</v>
@@ -1634,7 +1640,7 @@
       <c r="F7" s="19"/>
       <c r="G7" s="22"/>
       <c r="H7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -1645,14 +1651,14 @@
         <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="4"/>
       <c r="H8" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1676,12 +1682,12 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16">
         <f>(9+14+5)*6</f>
@@ -1690,7 +1696,7 @@
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17">
         <v>104</v>
@@ -1698,14 +1704,14 @@
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18">
         <f>SUM(D16:D17)</f>
         <v>272</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18">
         <f>SUM(Tabelle3[Effort Actual])</f>
@@ -1714,7 +1720,7 @@
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="F19" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="33">
         <f>D18-G18</f>
@@ -1734,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="131" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1791,7 +1797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -1799,19 +1805,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>5</v>
@@ -1827,10 +1833,10 @@
         <v>9</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1.2</v>
       </c>
@@ -1838,19 +1844,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>5</v>
@@ -1866,10 +1872,10 @@
         <v>3</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1.3</v>
       </c>
@@ -1877,16 +1883,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>24</v>
@@ -1904,10 +1910,10 @@
         <v>18</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1.4</v>
       </c>
@@ -1915,19 +1921,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>5</v>
@@ -1942,10 +1948,10 @@
         <v>3</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1.5</v>
       </c>
@@ -1953,13 +1959,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>24</v>
@@ -1980,10 +1986,10 @@
         <v>6</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1.6</v>
       </c>
@@ -1991,19 +1997,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>6</v>
@@ -2018,10 +2024,10 @@
         <v>6</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1.7</v>
       </c>
@@ -2029,13 +2035,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>27</v>
@@ -2056,10 +2062,10 @@
         <v>3</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>1.8</v>
       </c>
@@ -2067,13 +2073,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>22</v>
@@ -2094,10 +2100,10 @@
         <v>3</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="49" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>1.9</v>
       </c>
@@ -2105,13 +2111,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>24</v>
@@ -2133,10 +2139,10 @@
         <v>17</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="49" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>2.2000000000000002</v>
       </c>
@@ -2144,16 +2150,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>27</v>
@@ -2171,10 +2177,10 @@
         <v>3</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="41" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>2.21</v>
       </c>
@@ -2182,16 +2188,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>25</v>
@@ -2209,10 +2215,10 @@
         <v>14</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="41" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>3.1</v>
       </c>
@@ -2220,19 +2226,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>5</v>
@@ -2247,10 +2253,10 @@
         <v>10</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="38" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>2.2999999999999998</v>
       </c>
@@ -2258,13 +2264,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>27</v>
@@ -2285,10 +2291,10 @@
         <v>9</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>2.4</v>
       </c>
@@ -2296,13 +2302,13 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>22</v>
@@ -2323,10 +2329,10 @@
         <v>10</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>3.2</v>
       </c>
@@ -2334,19 +2340,19 @@
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>5</v>
@@ -2361,10 +2367,10 @@
         <v>11</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>2.6</v>
       </c>
@@ -2372,16 +2378,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>24</v>
@@ -2399,10 +2405,10 @@
         <v>3</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="31" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2.7</v>
       </c>
@@ -2410,16 +2416,16 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>24</v>
@@ -2437,10 +2443,10 @@
         <v>14</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>2.8</v>
       </c>
@@ -2448,19 +2454,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>5</v>
@@ -2475,10 +2481,10 @@
         <v>28</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>2.9</v>
       </c>
@@ -2486,16 +2492,16 @@
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>81</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>24</v>
@@ -2514,10 +2520,10 @@
         <v>12</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="40" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>5.0999999999999996</v>
       </c>
@@ -2525,16 +2531,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>83</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>24</v>
@@ -2553,7 +2559,7 @@
         <v>17</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -2564,19 +2570,19 @@
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>6</v>
@@ -2591,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -2602,16 +2608,16 @@
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>24</v>
@@ -2629,7 +2635,7 @@
         <v>8</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -2640,19 +2646,19 @@
         <v>3</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="E24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>5</v>
@@ -2667,7 +2673,7 @@
         <v>9</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
@@ -2678,13 +2684,13 @@
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>99</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>22</v>
@@ -2706,7 +2712,7 @@
         <v>32</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="32" x14ac:dyDescent="0.2">
@@ -2717,13 +2723,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>26</v>
@@ -2745,7 +2751,7 @@
         <v>20</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2787,13 +2793,13 @@
         <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -2811,7 +2817,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,7 +2835,7 @@
         <v>54</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2847,7 +2853,7 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -2865,7 +2871,7 @@
         <v>52</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -2883,7 +2889,7 @@
         <v>51</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -2901,7 +2907,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -2919,7 +2925,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2937,7 +2943,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2985,7 +2991,7 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80" x14ac:dyDescent="0.2">
@@ -3003,7 +3009,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -3021,7 +3027,7 @@
         <v>43</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3054,7 +3060,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3087,7 +3093,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3105,7 +3111,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3138,7 +3144,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3156,7 +3162,7 @@
         <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3174,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3252,7 +3258,7 @@
         <v>29</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3270,7 +3276,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3288,7 +3294,7 @@
         <v>27</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3501,7 +3507,7 @@
         <v>13</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -3564,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -3582,7 +3588,7 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -3600,7 +3606,7 @@
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3618,7 +3624,7 @@
         <v>6</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3636,7 +3642,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -3654,7 +3660,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -3672,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -3705,7 +3711,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -3723,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>